<commit_message>
Finalização DER e Diagrama de Classe
</commit_message>
<xml_diff>
--- a/Lista Atividades.xlsx
+++ b/Lista Atividades.xlsx
@@ -11,7 +11,7 @@
     <sheet name="config" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -751,7 +751,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -787,7 +787,7 @@
         <v>25</v>
       </c>
       <c r="D2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -801,7 +801,7 @@
         <v>26</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -815,7 +815,7 @@
         <v>26</v>
       </c>
       <c r="D4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -829,7 +829,7 @@
         <v>27</v>
       </c>
       <c r="D5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>